<commit_message>
Calcular inclusion y exclusion
</commit_message>
<xml_diff>
--- a/datosAsegurado.xlsx
+++ b/datosAsegurado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\RPA\RobotControlCumulos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4489984-B8D0-4D73-A966-3E6CE4A34AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B9C8B2-B3DA-40FF-82F9-D42E4658BEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="21">
-  <si>
-    <t>Emitido</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
   <si>
     <t>Sección</t>
   </si>
@@ -70,19 +67,31 @@
     <t>0106</t>
   </si>
   <si>
-    <t>CRISOL Y ENCARNACION FINANCIERA SOCIEDAD ANONIMA EMISORA DE CAPITAL ABIERTO</t>
+    <t>BANCO REGIONAL S.A.E.C.A.</t>
+  </si>
+  <si>
+    <t>7992852</t>
+  </si>
+  <si>
+    <t>8039671</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>BANCO REGIONAL S.A.E.C.A.</t>
-  </si>
-  <si>
-    <t>8265809</t>
-  </si>
-  <si>
-    <t>8291223</t>
+    <t>8106333</t>
+  </si>
+  <si>
+    <t>8163184</t>
+  </si>
+  <si>
+    <t>8198141</t>
+  </si>
+  <si>
+    <t>8252552</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -545,11 +554,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -568,87 +575,87 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="5">
-        <v>1444</v>
+        <v>4231</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>358</v>
+        <v>3</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" s="7">
-        <v>40718</v>
+        <v>42929</v>
       </c>
       <c r="I2" s="7">
-        <v>41084</v>
+        <v>43233</v>
       </c>
       <c r="J2" s="7">
-        <v>41084</v>
+        <v>43233</v>
       </c>
       <c r="K2" s="8">
-        <v>3984000</v>
+        <v>173712000</v>
       </c>
       <c r="L2" s="8">
-        <v>3984000</v>
+        <v>86856000</v>
       </c>
       <c r="M2" s="8">
-        <v>0</v>
+        <v>86856000</v>
       </c>
       <c r="N2" s="8">
         <v>0</v>
@@ -656,40 +663,40 @@
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5">
-        <v>1579</v>
+        <v>4982</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>254</v>
+        <v>7</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="7">
-        <v>40899</v>
+        <v>43236</v>
       </c>
       <c r="I3" s="7">
-        <v>41265</v>
+        <v>43601</v>
       </c>
       <c r="J3" s="7">
-        <v>41265</v>
+        <v>43601</v>
       </c>
       <c r="K3" s="8">
-        <v>14136000</v>
+        <v>173712000</v>
       </c>
       <c r="L3" s="8">
-        <v>14136000</v>
+        <v>86856000</v>
       </c>
       <c r="M3" s="8">
-        <v>0</v>
+        <v>86856000</v>
       </c>
       <c r="N3" s="8">
         <v>0</v>
@@ -697,40 +704,40 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5">
-        <v>1784</v>
+        <v>5823</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="7">
-        <v>41244</v>
+        <v>43601</v>
       </c>
       <c r="I4" s="7">
-        <v>41609</v>
+        <v>43606</v>
       </c>
       <c r="J4" s="7">
-        <v>41609</v>
+        <v>43606</v>
       </c>
       <c r="K4" s="8">
-        <v>14136000</v>
+        <v>173712000</v>
       </c>
       <c r="L4" s="8">
-        <v>7068000</v>
+        <v>86856000</v>
       </c>
       <c r="M4" s="8">
-        <v>7068000</v>
+        <v>86856000</v>
       </c>
       <c r="N4" s="8">
         <v>0</v>
@@ -738,40 +745,40 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
-        <v>2351</v>
+        <v>6055</v>
       </c>
       <c r="D5" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5">
-        <v>2180</v>
+        <v>22242</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="7">
-        <v>42005</v>
+        <v>43678</v>
       </c>
       <c r="I5" s="7">
-        <v>42035</v>
+        <v>43708</v>
       </c>
       <c r="J5" s="7">
-        <v>42035</v>
+        <v>43708</v>
       </c>
       <c r="K5" s="8">
-        <v>874968</v>
+        <v>119166</v>
       </c>
       <c r="L5" s="8">
-        <v>437484</v>
+        <v>59583</v>
       </c>
       <c r="M5" s="8">
-        <v>437484</v>
+        <v>59583</v>
       </c>
       <c r="N5" s="8">
         <v>0</v>
@@ -779,40 +786,40 @@
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5">
-        <v>2378</v>
+        <v>6099</v>
       </c>
       <c r="D6" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="5">
-        <v>2226</v>
+        <v>17912</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="7">
-        <v>42036</v>
+        <v>43709</v>
       </c>
       <c r="I6" s="7">
-        <v>42063</v>
+        <v>43738</v>
       </c>
       <c r="J6" s="7">
-        <v>42063</v>
+        <v>43738</v>
       </c>
       <c r="K6" s="8">
-        <v>623822</v>
+        <v>119166</v>
       </c>
       <c r="L6" s="8">
-        <v>311911</v>
+        <v>59583</v>
       </c>
       <c r="M6" s="8">
-        <v>311911</v>
+        <v>59583</v>
       </c>
       <c r="N6" s="8">
         <v>0</v>
@@ -820,40 +827,40 @@
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5">
-        <v>2413</v>
+        <v>6166</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5">
-        <v>2327</v>
+        <v>16763</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="7">
-        <v>42064</v>
+        <v>43739</v>
       </c>
       <c r="I7" s="7">
-        <v>42094</v>
+        <v>43769</v>
       </c>
       <c r="J7" s="7">
-        <v>42094</v>
+        <v>43769</v>
       </c>
       <c r="K7" s="8">
-        <v>354777</v>
+        <v>119167</v>
       </c>
       <c r="L7" s="8">
-        <v>177389</v>
+        <v>59584</v>
       </c>
       <c r="M7" s="8">
-        <v>177388</v>
+        <v>59583</v>
       </c>
       <c r="N7" s="8">
         <v>0</v>
@@ -861,40 +868,40 @@
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5">
-        <v>2432</v>
+        <v>5917</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>6810</v>
+        <v>7</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H8" s="7">
-        <v>42095</v>
+        <v>43628</v>
       </c>
       <c r="I8" s="7">
-        <v>42124</v>
+        <v>43980</v>
       </c>
       <c r="J8" s="7">
-        <v>42124</v>
+        <v>43980</v>
       </c>
       <c r="K8" s="8">
-        <v>376478</v>
+        <v>173712000</v>
       </c>
       <c r="L8" s="8">
-        <v>188239</v>
+        <v>86856000</v>
       </c>
       <c r="M8" s="8">
-        <v>188239</v>
+        <v>86856000</v>
       </c>
       <c r="N8" s="8">
         <v>0</v>
@@ -902,40 +909,40 @@
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5">
-        <v>2466</v>
+        <v>6614</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>6755</v>
+        <v>131</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H9" s="7">
-        <v>42125</v>
+        <v>43994</v>
       </c>
       <c r="I9" s="7">
-        <v>42155</v>
+        <v>44008</v>
       </c>
       <c r="J9" s="7">
-        <v>42155</v>
+        <v>44008</v>
       </c>
       <c r="K9" s="8">
-        <v>394104</v>
+        <v>173712000</v>
       </c>
       <c r="L9" s="8">
-        <v>197052</v>
+        <v>86856000</v>
       </c>
       <c r="M9" s="8">
-        <v>197052</v>
+        <v>86856000</v>
       </c>
       <c r="N9" s="8">
         <v>0</v>
@@ -943,40 +950,40 @@
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="5">
-        <v>2515</v>
+        <v>6773</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="5">
-        <v>3906</v>
+        <v>16202</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H10" s="7">
-        <v>42156</v>
+        <v>44044</v>
       </c>
       <c r="I10" s="7">
-        <v>42185</v>
+        <v>44074</v>
       </c>
       <c r="J10" s="7">
-        <v>42185</v>
+        <v>44074</v>
       </c>
       <c r="K10" s="8">
-        <v>263834</v>
+        <v>119166</v>
       </c>
       <c r="L10" s="8">
-        <v>131917</v>
+        <v>59583</v>
       </c>
       <c r="M10" s="8">
-        <v>131917</v>
+        <v>59583</v>
       </c>
       <c r="N10" s="8">
         <v>0</v>
@@ -984,40 +991,40 @@
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="5">
-        <v>2537</v>
+        <v>6838</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="5">
-        <v>4057</v>
+        <v>15987</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" s="7">
-        <v>42186</v>
+        <v>44075</v>
       </c>
       <c r="I11" s="7">
-        <v>42216</v>
+        <v>44104</v>
       </c>
       <c r="J11" s="7">
-        <v>42216</v>
+        <v>44104</v>
       </c>
       <c r="K11" s="8">
-        <v>292529</v>
+        <v>119166</v>
       </c>
       <c r="L11" s="8">
-        <v>146265</v>
+        <v>59583</v>
       </c>
       <c r="M11" s="8">
-        <v>146264</v>
+        <v>59583</v>
       </c>
       <c r="N11" s="8">
         <v>0</v>
@@ -1025,40 +1032,40 @@
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5">
-        <v>2696</v>
+        <v>6901</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="5">
-        <v>2562</v>
+        <v>15759</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="7">
-        <v>42248</v>
+        <v>44105</v>
       </c>
       <c r="I12" s="7">
-        <v>42277</v>
+        <v>44135</v>
       </c>
       <c r="J12" s="7">
-        <v>42277</v>
+        <v>44135</v>
       </c>
       <c r="K12" s="8">
-        <v>161072</v>
+        <v>119167</v>
       </c>
       <c r="L12" s="8">
-        <v>80536</v>
+        <v>59584</v>
       </c>
       <c r="M12" s="8">
-        <v>80536</v>
+        <v>59583</v>
       </c>
       <c r="N12" s="8">
         <v>0</v>
@@ -1066,40 +1073,40 @@
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5">
-        <v>2759</v>
+        <v>6714</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
       </c>
       <c r="E13" s="5">
-        <v>2444</v>
+        <v>3</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H13" s="7">
-        <v>42278</v>
+        <v>44028</v>
       </c>
       <c r="I13" s="7">
-        <v>42308</v>
+        <v>44316</v>
       </c>
       <c r="J13" s="7">
-        <v>42308</v>
+        <v>44316</v>
       </c>
       <c r="K13" s="8">
-        <v>169965</v>
+        <v>173712000</v>
       </c>
       <c r="L13" s="8">
-        <v>84983</v>
+        <v>86856000</v>
       </c>
       <c r="M13" s="8">
-        <v>84982</v>
+        <v>86856000</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -1107,40 +1114,40 @@
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>2835</v>
+        <v>6714</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="5">
-        <v>2321</v>
+        <v>3</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H14" s="7">
-        <v>42309</v>
+        <v>44028</v>
       </c>
       <c r="I14" s="7">
-        <v>42338</v>
+        <v>44316</v>
       </c>
       <c r="J14" s="7">
-        <v>42338</v>
+        <v>44316</v>
       </c>
       <c r="K14" s="8">
-        <v>131276</v>
+        <v>-173712000</v>
       </c>
       <c r="L14" s="8">
-        <v>65638</v>
+        <v>-86856000</v>
       </c>
       <c r="M14" s="8">
-        <v>65638</v>
+        <v>-86856000</v>
       </c>
       <c r="N14" s="8">
         <v>0</v>
@@ -1148,40 +1155,40 @@
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="5">
-        <v>2894</v>
+        <v>7540</v>
       </c>
       <c r="D15" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5">
-        <v>2241</v>
+        <v>14534</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H15" s="7">
-        <v>42339</v>
+        <v>44409</v>
       </c>
       <c r="I15" s="7">
-        <v>42369</v>
+        <v>44439</v>
       </c>
       <c r="J15" s="7">
-        <v>42369</v>
+        <v>44439</v>
       </c>
       <c r="K15" s="8">
-        <v>136799</v>
+        <v>119166</v>
       </c>
       <c r="L15" s="8">
-        <v>68400</v>
+        <v>59583</v>
       </c>
       <c r="M15" s="8">
-        <v>68399</v>
+        <v>59583</v>
       </c>
       <c r="N15" s="8">
         <v>0</v>
@@ -1189,40 +1196,40 @@
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5">
-        <v>2968</v>
+        <v>7615</v>
       </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="5">
-        <v>2170</v>
+        <v>14516</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H16" s="7">
-        <v>42370</v>
+        <v>44440</v>
       </c>
       <c r="I16" s="7">
-        <v>42400</v>
+        <v>44469</v>
       </c>
       <c r="J16" s="7">
-        <v>42400</v>
+        <v>44469</v>
       </c>
       <c r="K16" s="8">
-        <v>129217</v>
+        <v>119166</v>
       </c>
       <c r="L16" s="8">
-        <v>64609</v>
+        <v>59583</v>
       </c>
       <c r="M16" s="8">
-        <v>64608</v>
+        <v>59583</v>
       </c>
       <c r="N16" s="8">
         <v>0</v>
@@ -1230,40 +1237,40 @@
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="5">
-        <v>3054</v>
+        <v>7677</v>
       </c>
       <c r="D17" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="5">
-        <v>1888</v>
+        <v>14462</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H17" s="7">
-        <v>42401</v>
+        <v>44470</v>
       </c>
       <c r="I17" s="7">
-        <v>42429</v>
+        <v>44500</v>
       </c>
       <c r="J17" s="7">
-        <v>42429</v>
+        <v>44500</v>
       </c>
       <c r="K17" s="8">
-        <v>134838</v>
+        <v>130167</v>
       </c>
       <c r="L17" s="8">
-        <v>67419</v>
+        <v>65084</v>
       </c>
       <c r="M17" s="8">
-        <v>67419</v>
+        <v>65083</v>
       </c>
       <c r="N17" s="8">
         <v>0</v>
@@ -1271,40 +1278,40 @@
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
-        <v>3124</v>
+        <v>7297</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
       </c>
       <c r="E18" s="5">
-        <v>1842</v>
+        <v>4</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H18" s="7">
-        <v>42430</v>
+        <v>44306</v>
       </c>
       <c r="I18" s="7">
-        <v>42460</v>
+        <v>44666</v>
       </c>
       <c r="J18" s="7">
-        <v>42460</v>
+        <v>44666</v>
       </c>
       <c r="K18" s="8">
-        <v>145779</v>
+        <v>173712000</v>
       </c>
       <c r="L18" s="8">
-        <v>72890</v>
+        <v>86856000</v>
       </c>
       <c r="M18" s="8">
-        <v>72889</v>
+        <v>86856000</v>
       </c>
       <c r="N18" s="8">
         <v>0</v>
@@ -1312,40 +1319,40 @@
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="5">
-        <v>3222</v>
+        <v>8027</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <v>5035</v>
+        <v>91</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H19" s="7">
-        <v>42461</v>
+        <v>44671</v>
       </c>
       <c r="I19" s="7">
-        <v>42490</v>
+        <v>44676</v>
       </c>
       <c r="J19" s="7">
-        <v>42490</v>
+        <v>44676</v>
       </c>
       <c r="K19" s="8">
-        <v>151349</v>
+        <v>173712000</v>
       </c>
       <c r="L19" s="8">
-        <v>75675</v>
+        <v>86856000</v>
       </c>
       <c r="M19" s="8">
-        <v>75674</v>
+        <v>86856000</v>
       </c>
       <c r="N19" s="8">
         <v>0</v>
@@ -1353,40 +1360,40 @@
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="5">
-        <v>3311</v>
+        <v>8269</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <v>1677</v>
+        <v>13917</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H20" s="7">
-        <v>42491</v>
+        <v>44743</v>
       </c>
       <c r="I20" s="7">
-        <v>42521</v>
+        <v>44762</v>
       </c>
       <c r="J20" s="7">
-        <v>42521</v>
+        <v>44762</v>
       </c>
       <c r="K20" s="8">
-        <v>157637</v>
+        <v>144834</v>
       </c>
       <c r="L20" s="8">
-        <v>78819</v>
+        <v>72417</v>
       </c>
       <c r="M20" s="8">
-        <v>78818</v>
+        <v>72417</v>
       </c>
       <c r="N20" s="8">
         <v>0</v>
@@ -1394,40 +1401,40 @@
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="5">
-        <v>3351</v>
+        <v>8269</v>
       </c>
       <c r="D21" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="5">
-        <v>104</v>
+        <v>42148</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H21" s="7">
-        <v>42522</v>
+        <v>44763</v>
       </c>
       <c r="I21" s="7">
-        <v>42551</v>
+        <v>44792</v>
       </c>
       <c r="J21" s="7">
-        <v>42551</v>
+        <v>44792</v>
       </c>
       <c r="K21" s="8">
-        <v>164119</v>
+        <v>144834</v>
       </c>
       <c r="L21" s="8">
-        <v>82060</v>
+        <v>72417</v>
       </c>
       <c r="M21" s="8">
-        <v>82059</v>
+        <v>72417</v>
       </c>
       <c r="N21" s="8">
         <v>0</v>
@@ -1435,40 +1442,40 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="5">
-        <v>3430</v>
+        <v>8269</v>
       </c>
       <c r="D22" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22" s="5">
-        <v>1614</v>
+        <v>70763</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H22" s="7">
-        <v>42552</v>
+        <v>44793</v>
       </c>
       <c r="I22" s="7">
-        <v>42582</v>
+        <v>44824</v>
       </c>
       <c r="J22" s="7">
-        <v>42582</v>
+        <v>44824</v>
       </c>
       <c r="K22" s="8">
-        <v>170310</v>
+        <v>144833</v>
       </c>
       <c r="L22" s="8">
-        <v>85155</v>
+        <v>72417</v>
       </c>
       <c r="M22" s="8">
-        <v>85155</v>
+        <v>72416</v>
       </c>
       <c r="N22" s="8">
         <v>0</v>
@@ -1476,288 +1483,42 @@
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="5">
-        <v>2614</v>
+        <v>8070</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5">
-        <v>4016</v>
+        <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H23" s="7">
-        <v>42217</v>
+        <v>44672</v>
       </c>
       <c r="I23" s="7">
-        <v>42583</v>
+        <v>45028</v>
       </c>
       <c r="J23" s="7">
-        <v>42583</v>
+        <v>45028</v>
       </c>
       <c r="K23" s="8">
-        <v>236792</v>
+        <v>173712000</v>
       </c>
       <c r="L23" s="8">
-        <v>118396</v>
+        <v>86856000</v>
       </c>
       <c r="M23" s="8">
-        <v>118396</v>
+        <v>86856000</v>
       </c>
       <c r="N23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="5">
-        <v>3504</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1646</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="7">
-        <v>42583</v>
-      </c>
-      <c r="I24" s="7">
-        <v>42613</v>
-      </c>
-      <c r="J24" s="7">
-        <v>42613</v>
-      </c>
-      <c r="K24" s="8">
-        <v>176563</v>
-      </c>
-      <c r="L24" s="8">
-        <v>88282</v>
-      </c>
-      <c r="M24" s="8">
-        <v>88281</v>
-      </c>
-      <c r="N24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="5">
-        <v>3573</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1655</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="7">
-        <v>42614</v>
-      </c>
-      <c r="I25" s="7">
-        <v>42643</v>
-      </c>
-      <c r="J25" s="7">
-        <v>42643</v>
-      </c>
-      <c r="K25" s="8">
-        <v>190102</v>
-      </c>
-      <c r="L25" s="8">
-        <v>95051</v>
-      </c>
-      <c r="M25" s="8">
-        <v>95051</v>
-      </c>
-      <c r="N25" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="5">
-        <v>3639</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5">
-        <v>1637</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="7">
-        <v>42644</v>
-      </c>
-      <c r="I26" s="7">
-        <v>42674</v>
-      </c>
-      <c r="J26" s="7">
-        <v>42674</v>
-      </c>
-      <c r="K26" s="8">
-        <v>203068</v>
-      </c>
-      <c r="L26" s="8">
-        <v>101534</v>
-      </c>
-      <c r="M26" s="8">
-        <v>101534</v>
-      </c>
-      <c r="N26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="5">
-        <v>3726</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5">
-        <v>1545</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="7">
-        <v>42675</v>
-      </c>
-      <c r="I27" s="7">
-        <v>42704</v>
-      </c>
-      <c r="J27" s="7">
-        <v>42704</v>
-      </c>
-      <c r="K27" s="8">
-        <v>216141</v>
-      </c>
-      <c r="L27" s="8">
-        <v>108071</v>
-      </c>
-      <c r="M27" s="8">
-        <v>108070</v>
-      </c>
-      <c r="N27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="5">
-        <v>8241</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5">
-        <v>9</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="7">
-        <v>44754</v>
-      </c>
-      <c r="I28" s="7">
-        <v>45118</v>
-      </c>
-      <c r="J28" s="7">
-        <v>45118</v>
-      </c>
-      <c r="K28" s="8">
-        <v>21000000</v>
-      </c>
-      <c r="L28" s="8">
-        <v>10500000</v>
-      </c>
-      <c r="M28" s="8">
-        <v>10500000</v>
-      </c>
-      <c r="N28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="5">
-        <v>8581</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5">
-        <v>259</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="7">
-        <v>44914</v>
-      </c>
-      <c r="I29" s="7">
-        <v>45278</v>
-      </c>
-      <c r="J29" s="7">
-        <v>45278</v>
-      </c>
-      <c r="K29" s="8">
-        <v>2800000</v>
-      </c>
-      <c r="L29" s="8">
-        <v>1400000</v>
-      </c>
-      <c r="M29" s="8">
-        <v>1400000</v>
-      </c>
-      <c r="N29" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>